<commit_message>
cambios trazabilidad y la base de datos
</commit_message>
<xml_diff>
--- a/PhpProjectVenta/docs/30-august-2017/TrazabilidadVentas.xlsx
+++ b/PhpProjectVenta/docs/30-august-2017/TrazabilidadVentas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="390" windowWidth="19875" windowHeight="7725" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="390" windowWidth="19875" windowHeight="7725"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -845,7 +845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -853,7 +853,7 @@
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
     <col min="7" max="7" width="23.42578125" customWidth="1"/>
     <col min="9" max="9" width="25.5703125" customWidth="1"/>
     <col min="11" max="11" width="12" customWidth="1"/>
@@ -1159,7 +1159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>

</xml_diff>